<commit_message>
Added Registrering and Omregistrering to documentation.
</commit_message>
<xml_diff>
--- a/INT0009.Sesam.Events/Src/Files/INT0009.Sesam.Events.maps.xlsx
+++ b/INT0009.Sesam.Events/Src/Files/INT0009.Sesam.Events.maps.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peasb031\Documents\BizTalk Ladok\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonam895\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KurstillfalleTillStatusEvent" sheetId="6" r:id="rId1"/>
     <sheet name="KurspaketeringUppdateradEvent" sheetId="7" r:id="rId2"/>
+    <sheet name="RegistreringEnvelope" sheetId="10" r:id="rId3"/>
+    <sheet name="OmregistreringEnvelope" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="47">
   <si>
     <t>Från</t>
   </si>
@@ -100,12 +102,78 @@
   </si>
   <si>
     <t>Programkod</t>
+  </si>
+  <si>
+    <t>Mappning: RegistreringEnvelope_to_PersonEvent</t>
+  </si>
+  <si>
+    <t>Target: http://INT0009.Sesam.Events.Schemas.Sesam.PersonEvent</t>
+  </si>
+  <si>
+    <t>/PersonEvent</t>
+  </si>
+  <si>
+    <t>Mappning: OmregistreringEnvelope_to_PersonEvent</t>
+  </si>
+  <si>
+    <t>Fast värde "R"</t>
+  </si>
+  <si>
+    <t>Personnummer</t>
+  </si>
+  <si>
+    <t>/Student/Personnummer</t>
+  </si>
+  <si>
+    <t>Efternamn</t>
+  </si>
+  <si>
+    <t>Fornamn</t>
+  </si>
+  <si>
+    <t>Startdatum</t>
+  </si>
+  <si>
+    <t>Slutdatum</t>
+  </si>
+  <si>
+    <t>StartterminForKurs</t>
+  </si>
+  <si>
+    <t>Programslut</t>
+  </si>
+  <si>
+    <t>/Student/Efternamn</t>
+  </si>
+  <si>
+    <t>/Student/Fornamn</t>
+  </si>
+  <si>
+    <t>/RegistreringEvent/StudieperiodStart</t>
+  </si>
+  <si>
+    <t>/RegistreringEvent/StudieperiodSlut</t>
+  </si>
+  <si>
+    <t>Välj den Utbildningsinstans som har samma UID som /RegistreringEvent/UtbildningsinstansUID</t>
+  </si>
+  <si>
+    <t>Om Inomkurspaketeringstillfalle finns så matcha KurspaketeringstillfalleUID mot Utbildningstillfalle/Uid. Ta Utbildningstillfällets UID och matcha mot Utbildningsinstans/UID. Ta sedan utbildningsinstansens Utbildningskod.</t>
+  </si>
+  <si>
+    <t>Ta fyrsiffrigt år. Lägg på "1" i slutet om månaden är jan-jun. Annars lägg på "2"</t>
+  </si>
+  <si>
+    <t>/OmregistreringEvent/StudieperiodStart</t>
+  </si>
+  <si>
+    <t>/OmregistreringEvent/StudieperiodSlut</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,7 +230,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -196,10 +264,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Dekorfärg1" xfId="1" builtinId="29"/>
-    <cellStyle name="Dekorfärg5" xfId="2" builtinId="45"/>
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Accent5" xfId="2" builtinId="45"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -484,21 +556,21 @@
       <selection activeCell="A17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="13"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
@@ -508,7 +580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -522,13 +594,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>14</v>
       </c>
@@ -536,7 +608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -544,12 +616,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>17</v>
       </c>
@@ -560,7 +632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>18</v>
       </c>
@@ -568,7 +640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>15</v>
       </c>
@@ -576,31 +648,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="C22" s="5"/>
       <c r="D22" s="11"/>
@@ -619,25 +691,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="13"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
@@ -647,7 +719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -661,13 +733,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>21</v>
       </c>
@@ -675,7 +747,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -683,12 +755,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>17</v>
       </c>
@@ -699,37 +771,392 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" s="12"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="13"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="13"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="C22" s="5"/>
       <c r="D22" s="11"/>

</xml_diff>